<commit_message>
Deploying to gh-pages from @ Healthedata1/USCDI4-Sandbox@cc0d6b03de903db85c68c9d177625950aaff22bd 🚀
</commit_message>
<xml_diff>
--- a/observations-summary.xlsx
+++ b/observations-summary.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="22">
   <si>
     <t>Profile</t>
   </si>
@@ -45,6 +45,39 @@
   </si>
   <si>
     <t>Method</t>
+  </si>
+  <si>
+    <t>us-core-average-blood-pressure</t>
+  </si>
+  <si>
+    <t>US Core Average Blood Pressure Profile</t>
+  </si>
+  <si>
+    <t>null#vital-signs</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>LOINC#96607-7</t>
+  </si>
+  <si>
+    <t>dateTimeĵ, Periodĵ</t>
+  </si>
+  <si>
+    <t>Quantityĵ, CodeableConceptĵ, stringĵ, booleanĵ, integerĵ, Rangeĵ, Ratioĵ, SampledDataĵ, timeĵ, dateTimeĵ, Periodĵ</t>
+  </si>
+  <si>
+    <t>optional</t>
+  </si>
+  <si>
+    <t>LOINC#96608-5</t>
+  </si>
+  <si>
+    <t>Quantityĵ</t>
+  </si>
+  <si>
+    <t>LOINC#96609-3</t>
   </si>
 </sst>
 </file>
@@ -178,7 +211,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -219,6 +252,111 @@
         <v>10</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="s" s="2">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s" s="2">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s" s="2">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s" s="2">
+        <v>15</v>
+      </c>
+      <c r="F2" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="G2" t="s" s="2">
+        <v>16</v>
+      </c>
+      <c r="H2" t="s" s="2">
+        <v>17</v>
+      </c>
+      <c r="I2" t="s" s="2">
+        <v>18</v>
+      </c>
+      <c r="J2" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="K2" t="s" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s" s="2">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="F3" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="G3" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="H3" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="I3" t="s" s="2">
+        <v>18</v>
+      </c>
+      <c r="J3" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="K3" t="s" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s" s="2">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="E4" t="s" s="2">
+        <v>21</v>
+      </c>
+      <c r="F4" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="G4" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="H4" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="I4" t="s" s="2">
+        <v>18</v>
+      </c>
+      <c r="J4" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="K4" t="s" s="2">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ Healthedata1/USCDI4-Sandbox@ebf12a38bf5ca393f44c6a5c427f6ad39221c377 🚀
</commit_message>
<xml_diff>
--- a/observations-summary.xlsx
+++ b/observations-summary.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="27">
   <si>
     <t>Profile</t>
   </si>
@@ -53,7 +53,7 @@
     <t>US Core Average Blood Pressure Profile</t>
   </si>
   <si>
-    <t>null#vital-signs</t>
+    <t>Observation Category Codes#vital-signs</t>
   </si>
   <si>
     <t/>
@@ -78,6 +78,21 @@
   </si>
   <si>
     <t>LOINC#96609-3</t>
+  </si>
+  <si>
+    <t>us-core-observation-lab</t>
+  </si>
+  <si>
+    <t>US Core Laboratory Result Observation Profile</t>
+  </si>
+  <si>
+    <t>Observation Category Codes#laboratory</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/core/ValueSet/us-core-laboratory-test-codes (extensible)</t>
+  </si>
+  <si>
+    <t>dateTimeĵ, Periodĵ, Timingĵ, instantĵ</t>
   </si>
 </sst>
 </file>
@@ -211,7 +226,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -357,6 +372,41 @@
         <v>14</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="s" s="2">
+        <v>22</v>
+      </c>
+      <c r="B5" t="s" s="2">
+        <v>23</v>
+      </c>
+      <c r="C5" t="s" s="2">
+        <v>24</v>
+      </c>
+      <c r="D5" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="E5" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="F5" t="s" s="2">
+        <v>25</v>
+      </c>
+      <c r="G5" t="s" s="2">
+        <v>26</v>
+      </c>
+      <c r="H5" t="s" s="2">
+        <v>17</v>
+      </c>
+      <c r="I5" t="s" s="2">
+        <v>18</v>
+      </c>
+      <c r="J5" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="K5" t="s" s="2">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ Healthedata1/USCDI4-Sandbox@2bf753f3d0a9bdf5998e17093448378fa722e76c 🚀
</commit_message>
<xml_diff>
--- a/observations-summary.xlsx
+++ b/observations-summary.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="22">
   <si>
     <t>Profile</t>
   </si>
@@ -53,13 +53,13 @@
     <t>US Core Average Blood Pressure Profile</t>
   </si>
   <si>
-    <t>Observation Category Codes#vital-signs</t>
+    <t>null#vital-signs</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
-    <t>LOINC#96607-7</t>
+    <t>LOINC#85354-9, LOINC#96607-7</t>
   </si>
   <si>
     <t>dateTimeĵ, Periodĵ</t>
@@ -71,49 +71,13 @@
     <t>optional</t>
   </si>
   <si>
-    <t>LOINC#96608-5</t>
+    <t>LOINC#8480-6, LOINC#96608-5</t>
   </si>
   <si>
     <t>Quantityĵ</t>
   </si>
   <si>
-    <t>LOINC#96609-3</t>
-  </si>
-  <si>
-    <t>us-core-care-experience-preference</t>
-  </si>
-  <si>
-    <t>US Core Care Experience Preference Profile</t>
-  </si>
-  <si>
-    <t>US Core Category#care-experience-preference</t>
-  </si>
-  <si>
-    <t>LOINC#95541-9</t>
-  </si>
-  <si>
-    <t>dateTimeĵ, Periodĵ, Timingĵ, instantĵ</t>
-  </si>
-  <si>
-    <t>us-core-observation-lab</t>
-  </si>
-  <si>
-    <t>US Core Laboratory Result Observation Profile</t>
-  </si>
-  <si>
-    <t>Observation Category Codes#laboratory</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/core/ValueSet/us-core-laboratory-test-codes (extensible)</t>
-  </si>
-  <si>
-    <t>us-core-treatment-intervention-preference</t>
-  </si>
-  <si>
-    <t>US Core Treatment Intervention Preference Profile</t>
-  </si>
-  <si>
-    <t>US Core Category#treatment-intervention-preference</t>
+    <t>LOINC#8462-4, LOINC#96609-3</t>
   </si>
 </sst>
 </file>
@@ -247,7 +211,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -393,111 +357,6 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="s" s="2">
-        <v>22</v>
-      </c>
-      <c r="B5" t="s" s="2">
-        <v>23</v>
-      </c>
-      <c r="C5" t="s" s="2">
-        <v>24</v>
-      </c>
-      <c r="D5" t="s" s="2">
-        <v>14</v>
-      </c>
-      <c r="E5" t="s" s="2">
-        <v>25</v>
-      </c>
-      <c r="F5" t="s" s="2">
-        <v>14</v>
-      </c>
-      <c r="G5" t="s" s="2">
-        <v>26</v>
-      </c>
-      <c r="H5" t="s" s="2">
-        <v>17</v>
-      </c>
-      <c r="I5" t="s" s="2">
-        <v>18</v>
-      </c>
-      <c r="J5" t="s" s="2">
-        <v>14</v>
-      </c>
-      <c r="K5" t="s" s="2">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="B6" t="s" s="2">
-        <v>28</v>
-      </c>
-      <c r="C6" t="s" s="2">
-        <v>29</v>
-      </c>
-      <c r="D6" t="s" s="2">
-        <v>14</v>
-      </c>
-      <c r="E6" t="s" s="2">
-        <v>14</v>
-      </c>
-      <c r="F6" t="s" s="2">
-        <v>30</v>
-      </c>
-      <c r="G6" t="s" s="2">
-        <v>26</v>
-      </c>
-      <c r="H6" t="s" s="2">
-        <v>17</v>
-      </c>
-      <c r="I6" t="s" s="2">
-        <v>18</v>
-      </c>
-      <c r="J6" t="s" s="2">
-        <v>14</v>
-      </c>
-      <c r="K6" t="s" s="2">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s" s="2">
-        <v>31</v>
-      </c>
-      <c r="B7" t="s" s="2">
-        <v>32</v>
-      </c>
-      <c r="C7" t="s" s="2">
-        <v>33</v>
-      </c>
-      <c r="D7" t="s" s="2">
-        <v>14</v>
-      </c>
-      <c r="E7" t="s" s="2">
-        <v>33</v>
-      </c>
-      <c r="F7" t="s" s="2">
-        <v>14</v>
-      </c>
-      <c r="G7" t="s" s="2">
-        <v>26</v>
-      </c>
-      <c r="H7" t="s" s="2">
-        <v>17</v>
-      </c>
-      <c r="I7" t="s" s="2">
-        <v>18</v>
-      </c>
-      <c r="J7" t="s" s="2">
-        <v>14</v>
-      </c>
-      <c r="K7" t="s" s="2">
-        <v>14</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>